<commit_message>
Add category variable to csv and excel
</commit_message>
<xml_diff>
--- a/data/raw/dp.xlsx
+++ b/data/raw/dp.xlsx
@@ -5,36 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c8b45fca29679de1/Bureau/CEU/DA1/DA_team_project/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrae\OneDrive\Bureau\CEU\DA1\DA_team_project\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{98BB67F7-FEF8-423D-BA9E-5DDDE83ACD31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A9CBDB87-C1F3-4014-BE9E-5807D5DA6124}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C3C45F-980C-47F1-AC3B-7626BF472E70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{766EA92D-B2ED-445F-A457-B360843033AA}"/>
   </bookViews>
   <sheets>
     <sheet name="pizza_data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="146">
   <si>
     <t>id</t>
   </si>
@@ -445,13 +436,40 @@
   </si>
   <si>
     <t>Budapest, Bécsi út 65, 1036</t>
+  </si>
+  <si>
+    <t>Type_beverage</t>
+  </si>
+  <si>
+    <t>Pepsi</t>
+  </si>
+  <si>
+    <t>Coca cola</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>Beer</t>
+  </si>
+  <si>
+    <t>Lemonade</t>
+  </si>
+  <si>
+    <t>beer</t>
+  </si>
+  <si>
+    <t>beverage_vategory</t>
+  </si>
+  <si>
+    <t>Soft</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -521,13 +539,31 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -543,7 +579,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -602,12 +638,52 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <sz val="11"/>
@@ -615,6 +691,30 @@
       </font>
       <fill>
         <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -816,6 +916,18 @@
     </dxf>
     <dxf>
       <font>
+        <sz val="11"/>
+        <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -829,18 +941,6 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -860,24 +960,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE032252-B055-49E5-878D-3C0D3EF345CB}" name="Table1" displayName="Table1" ref="A2:O42" totalsRowShown="0" headerRowDxfId="15" dataDxfId="16">
-  <autoFilter ref="A2:O42" xr:uid="{2F480E6D-F058-4B7F-BCA4-FF1B5313A4E9}"/>
-  <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{62FD63ED-5730-457B-9C70-D636FB81702D}" name="id" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{764ECBEB-3741-4858-ABC7-7787BF320D14}" name="category" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{9E60E653-E5BB-4CFC-982B-B22A3231963C}" name="name" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{9E209C77-4346-4C98-A432-EF586AC6BF65}" name="website" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{67F863AE-7B4B-4F53-93AA-8645E0F1FA9A}" name="address" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{5D62F0A8-D6D5-4671-8E98-59239E24F31F}" name="long" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{03051C37-A905-452A-B0B9-30076CE6E202}" name="lat" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{D772B9A9-1453-47F5-9266-8142B5565C9C}" name="rating_google" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{97E97AF2-0307-461D-A157-B6C87E9CC121}" name="no_ratings" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{71F3B115-9733-499B-8D89-6CE6B8A04CAC}" name="open" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{B8F4CA71-17F0-43BB-9482-527D8DA9135D}" name="close" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{B8C4AE82-451F-4721-9D5B-27F34ADCA3A6}" name="no_pizza" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{94537314-779E-4EC1-B6EB-1075577AD62A}" name="price_marg" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{F3D28ABE-84C6-4FB3-921A-4D4B96166578}" name="price_bev" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{4D666295-B978-4A7E-99C4-FC250498E7CB}" name="price_del" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE032252-B055-49E5-878D-3C0D3EF345CB}" name="Table1" displayName="Table1" ref="A2:Q42" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A2:Q42" xr:uid="{2F480E6D-F058-4B7F-BCA4-FF1B5313A4E9}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{62FD63ED-5730-457B-9C70-D636FB81702D}" name="id" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{764ECBEB-3741-4858-ABC7-7787BF320D14}" name="category" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{9E60E653-E5BB-4CFC-982B-B22A3231963C}" name="name" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{9E209C77-4346-4C98-A432-EF586AC6BF65}" name="website" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{67F863AE-7B4B-4F53-93AA-8645E0F1FA9A}" name="address" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{5D62F0A8-D6D5-4671-8E98-59239E24F31F}" name="long" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{03051C37-A905-452A-B0B9-30076CE6E202}" name="lat" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{D772B9A9-1453-47F5-9266-8142B5565C9C}" name="rating_google" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{97E97AF2-0307-461D-A157-B6C87E9CC121}" name="no_ratings" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{71F3B115-9733-499B-8D89-6CE6B8A04CAC}" name="open" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{B8F4CA71-17F0-43BB-9482-527D8DA9135D}" name="close" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{B8C4AE82-451F-4721-9D5B-27F34ADCA3A6}" name="no_pizza" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{94537314-779E-4EC1-B6EB-1075577AD62A}" name="price_marg" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{F3D28ABE-84C6-4FB3-921A-4D4B96166578}" name="price_bev" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{337193B2-EC13-4730-B679-C77AE6EE89F2}" name="Type_beverage" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{5E1A9419-62B7-402F-AD43-E7FCEEAB6B6F}" name="beverage_vategory" dataDxfId="0"/>
+    <tableColumn id="16" xr3:uid="{4D666295-B978-4A7E-99C4-FC250498E7CB}" name="price_del" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1180,11 +1282,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06386B2C-4DEE-4A1C-8D12-67C699609A89}">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1200,13 +1302,15 @@
     <col min="10" max="10" width="14" style="1" customWidth="1"/>
     <col min="11" max="12" width="13" style="1" customWidth="1"/>
     <col min="13" max="13" width="14.109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="23.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" hidden="1">
+    <row r="1" spans="1:17" hidden="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1249,11 +1353,11 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.6">
+    <row r="2" spans="1:17" ht="15.6">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1297,10 +1401,16 @@
         <v>13</v>
       </c>
       <c r="O2" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:17">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -1343,11 +1453,17 @@
       <c r="N3" s="7">
         <v>400</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="P3" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q3" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:17">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -1390,11 +1506,17 @@
       <c r="N4" s="7">
         <v>350</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="O4" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q4" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:17">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -1434,14 +1556,20 @@
       <c r="M5" s="16">
         <v>2640</v>
       </c>
-      <c r="N5" s="16">
-        <v>1090</v>
-      </c>
-      <c r="O5" s="7" t="s">
+      <c r="N5" s="22">
+        <v>350</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="P5" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q5" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:17">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -1484,11 +1612,17 @@
       <c r="N6" s="7">
         <v>490</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="O6" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="P6" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q6" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:17">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -1498,7 +1632,7 @@
       <c r="C7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="23" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -1531,11 +1665,17 @@
       <c r="N7" s="7">
         <v>950</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="O7" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="P7" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q7" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:17">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -1578,11 +1718,17 @@
       <c r="N8" s="7">
         <v>860</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="O8" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="P8" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q8" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:17">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -1592,7 +1738,7 @@
       <c r="C9" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="23" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="8" t="s">
@@ -1622,14 +1768,20 @@
       <c r="M9" s="7">
         <v>1701</v>
       </c>
-      <c r="N9" s="7">
-        <v>280</v>
-      </c>
-      <c r="O9" s="7" t="s">
+      <c r="N9" s="24">
+        <v>360</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q9" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:17">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -1672,11 +1824,17 @@
       <c r="N10" s="7">
         <v>890</v>
       </c>
-      <c r="O10" s="7" t="s">
+      <c r="O10" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="P10" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q10" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:17">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -1719,11 +1877,17 @@
       <c r="N11" s="7">
         <v>500</v>
       </c>
-      <c r="O11" s="7" t="s">
+      <c r="O11" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="P11" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q11" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:17">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -1766,11 +1930,17 @@
       <c r="N12" s="7">
         <v>400</v>
       </c>
-      <c r="O12" s="7" t="s">
+      <c r="O12" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="P12" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q12" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:17">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -1810,14 +1980,20 @@
       <c r="M13" s="7">
         <v>1850</v>
       </c>
-      <c r="N13" s="7">
-        <v>650</v>
-      </c>
-      <c r="O13" s="7" t="s">
+      <c r="N13" s="21">
+        <v>500</v>
+      </c>
+      <c r="O13" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="P13" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q13" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:17">
       <c r="A14" s="7">
         <v>12</v>
       </c>
@@ -1860,11 +2036,17 @@
       <c r="N14" s="7">
         <v>790</v>
       </c>
-      <c r="O14" s="7" t="s">
+      <c r="O14" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="P14" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q14" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:17">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -1907,11 +2089,17 @@
       <c r="N15" s="7">
         <v>690</v>
       </c>
-      <c r="O15" s="7" t="s">
+      <c r="O15" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="P15" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q15" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:17">
       <c r="A16" s="7">
         <v>14</v>
       </c>
@@ -1954,11 +2142,17 @@
       <c r="N16" s="7">
         <v>950</v>
       </c>
-      <c r="O16" s="7" t="s">
+      <c r="O16" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="P16" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q16" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:17">
       <c r="A17" s="7">
         <v>15</v>
       </c>
@@ -2001,11 +2195,17 @@
       <c r="N17" s="7">
         <v>890</v>
       </c>
-      <c r="O17" s="7" t="s">
+      <c r="O17" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="P17" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q17" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:17">
       <c r="A18" s="7">
         <v>16</v>
       </c>
@@ -2045,14 +2245,20 @@
       <c r="M18" s="7">
         <v>2290</v>
       </c>
-      <c r="N18" s="7">
-        <v>790</v>
-      </c>
-      <c r="O18" s="7" t="s">
+      <c r="N18" s="21">
+        <v>890</v>
+      </c>
+      <c r="O18" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="P18" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q18" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:17">
       <c r="A19" s="7">
         <v>17</v>
       </c>
@@ -2095,11 +2301,17 @@
       <c r="N19" s="7">
         <v>550</v>
       </c>
-      <c r="O19" s="7" t="s">
+      <c r="O19" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="P19" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q19" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:17">
       <c r="A20" s="7">
         <v>18</v>
       </c>
@@ -2142,11 +2354,17 @@
       <c r="N20" s="7">
         <v>600</v>
       </c>
-      <c r="O20" s="7" t="s">
+      <c r="O20" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="P20" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q20" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:17">
       <c r="A21" s="7">
         <v>19</v>
       </c>
@@ -2189,11 +2407,17 @@
       <c r="N21" s="7">
         <v>980</v>
       </c>
-      <c r="O21" s="7" t="s">
+      <c r="O21" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="P21" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q21" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:17">
       <c r="A22" s="7">
         <v>20</v>
       </c>
@@ -2236,11 +2460,17 @@
       <c r="N22" s="7">
         <v>800</v>
       </c>
-      <c r="O22" s="7" t="s">
+      <c r="O22" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="P22" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q22" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:17">
       <c r="A23" s="19">
         <v>21</v>
       </c>
@@ -2283,11 +2513,17 @@
       <c r="N23" s="7">
         <v>500</v>
       </c>
-      <c r="O23" s="7">
+      <c r="O23" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="P23" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q23" s="7">
         <v>490</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:17">
       <c r="A24" s="19">
         <v>22</v>
       </c>
@@ -2330,11 +2566,17 @@
       <c r="N24" s="7">
         <v>530</v>
       </c>
-      <c r="O24" s="7">
+      <c r="O24" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="P24" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q24" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:17">
       <c r="A25" s="19">
         <v>23</v>
       </c>
@@ -2374,14 +2616,20 @@
       <c r="M25" s="7">
         <v>1890</v>
       </c>
-      <c r="N25" s="7">
-        <v>400</v>
-      </c>
-      <c r="O25" s="7">
+      <c r="N25" s="21">
+        <v>350</v>
+      </c>
+      <c r="O25" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="P25" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q25" s="7">
         <v>490</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:17">
       <c r="A26" s="19">
         <v>24</v>
       </c>
@@ -2424,11 +2672,17 @@
       <c r="N26" s="7">
         <v>590</v>
       </c>
-      <c r="O26" s="7">
+      <c r="O26" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="P26" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q26" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:17">
       <c r="A27" s="19">
         <v>25</v>
       </c>
@@ -2471,11 +2725,17 @@
       <c r="N27" s="7">
         <v>590</v>
       </c>
-      <c r="O27" s="7">
+      <c r="O27" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="P27" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q27" s="7">
         <v>500</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:17">
       <c r="A28" s="19">
         <v>26</v>
       </c>
@@ -2518,11 +2778,17 @@
       <c r="N28" s="7">
         <v>400</v>
       </c>
-      <c r="O28" s="7">
+      <c r="O28" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="P28" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q28" s="7">
         <v>490</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:17">
       <c r="A29" s="19">
         <v>27</v>
       </c>
@@ -2565,11 +2831,17 @@
       <c r="N29" s="7">
         <v>490</v>
       </c>
-      <c r="O29" s="7">
+      <c r="O29" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="P29" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q29" s="7">
         <v>499</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:17">
       <c r="A30" s="19">
         <v>28</v>
       </c>
@@ -2612,11 +2884,17 @@
       <c r="N30" s="7">
         <v>400</v>
       </c>
-      <c r="O30" s="7">
+      <c r="O30" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="P30" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q30" s="7">
         <v>490</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:17">
       <c r="A31" s="19">
         <v>29</v>
       </c>
@@ -2659,11 +2937,17 @@
       <c r="N31" s="7">
         <v>420</v>
       </c>
-      <c r="O31" s="7">
+      <c r="O31" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="P31" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q31" s="7">
         <v>490</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:17">
       <c r="A32" s="19">
         <v>30</v>
       </c>
@@ -2706,11 +2990,17 @@
       <c r="N32" s="7">
         <v>490</v>
       </c>
-      <c r="O32" s="7">
+      <c r="O32" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="P32" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q32" s="7">
         <v>490</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:17">
       <c r="A33" s="19">
         <v>31</v>
       </c>
@@ -2753,11 +3043,17 @@
       <c r="N33" s="7">
         <v>350</v>
       </c>
-      <c r="O33" s="7">
+      <c r="O33" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="P33" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q33" s="7">
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:17">
       <c r="A34" s="19">
         <v>32</v>
       </c>
@@ -2800,11 +3096,17 @@
       <c r="N34" s="7">
         <v>390</v>
       </c>
-      <c r="O34" s="7">
+      <c r="O34" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="P34" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q34" s="7">
         <v>490</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:17">
       <c r="A35" s="19">
         <v>33</v>
       </c>
@@ -2847,11 +3149,17 @@
       <c r="N35" s="7">
         <v>390</v>
       </c>
-      <c r="O35" s="7">
+      <c r="O35" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="P35" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q35" s="7">
         <v>290</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:17">
       <c r="A36" s="19">
         <v>34</v>
       </c>
@@ -2894,11 +3202,17 @@
       <c r="N36" s="7">
         <v>450</v>
       </c>
-      <c r="O36" s="7">
+      <c r="O36" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="P36" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q36" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:17">
       <c r="A37" s="19">
         <v>35</v>
       </c>
@@ -2941,11 +3255,17 @@
       <c r="N37" s="7">
         <v>400</v>
       </c>
-      <c r="O37" s="7">
+      <c r="O37" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="P37" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q37" s="7">
         <v>490</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:17">
       <c r="A38" s="19">
         <v>36</v>
       </c>
@@ -2988,11 +3308,17 @@
       <c r="N38" s="7">
         <v>450</v>
       </c>
-      <c r="O38" s="7">
+      <c r="O38" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="P38" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q38" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:17">
       <c r="A39" s="19">
         <v>37</v>
       </c>
@@ -3035,11 +3361,17 @@
       <c r="N39" s="7">
         <v>650</v>
       </c>
-      <c r="O39" s="7">
+      <c r="O39" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="P39" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q39" s="7">
         <v>490</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:17">
       <c r="A40" s="19">
         <v>38</v>
       </c>
@@ -3082,11 +3414,17 @@
       <c r="N40" s="7">
         <v>350</v>
       </c>
-      <c r="O40" s="7">
+      <c r="O40" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="P40" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q40" s="7">
         <v>499</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:17">
       <c r="A41" s="19">
         <v>39</v>
       </c>
@@ -3129,11 +3467,17 @@
       <c r="N41" s="7">
         <v>350</v>
       </c>
-      <c r="O41" s="7">
+      <c r="O41" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="P41" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q41" s="7">
         <v>499</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:17">
       <c r="A42" s="19">
         <v>40</v>
       </c>
@@ -3176,7 +3520,13 @@
       <c r="N42" s="7">
         <v>450</v>
       </c>
-      <c r="O42" s="7">
+      <c r="O42" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="P42" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q42" s="7">
         <v>899</v>
       </c>
     </row>
@@ -3191,11 +3541,13 @@
     <hyperlink ref="D8" r:id="rId7" xr:uid="{FD5D1918-EAB8-4096-A4EF-570F46E76DD5}"/>
     <hyperlink ref="D41" r:id="rId8" xr:uid="{00EA0077-68CC-4262-8269-37031FCCA403}"/>
     <hyperlink ref="D40" r:id="rId9" xr:uid="{2E76C2E2-4EAB-4596-8F70-D438D8647BEA}"/>
+    <hyperlink ref="D7" r:id="rId10" xr:uid="{477C6FBA-8225-4095-B25B-AE5E5867FD9E}"/>
+    <hyperlink ref="D9" r:id="rId11" xr:uid="{5D6848DB-41DE-4A32-B696-4F8EF087BD29}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>